<commit_message>
work on the "spike in" signatures
</commit_message>
<xml_diff>
--- a/comments-on-New_Table_S4.xlsx
+++ b/comments-on-New_Table_S4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve rozen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\non-M\github\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25397F4A-5958-4460-A8B3-F0248706283C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2BC716-4C39-4EE3-9DA4-FECA6AB5261C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-64110" yWindow="-3450" windowWidth="38620" windowHeight="21220" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-56940" yWindow="-1480" windowWidth="28770" windowHeight="15300" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="106">
   <si>
     <t>ID5</t>
   </si>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>Signature missed by SigProfilerExtractor in 4 runs</t>
-  </si>
-  <si>
-    <t>Signature missed by mSigHdp in all 5 runs</t>
   </si>
   <si>
     <t>Active tumors</t>
@@ -406,7 +403,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -477,12 +474,6 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -690,15 +681,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -738,9 +720,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,6 +732,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1303,10 +1294,10 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="54"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -1418,10 +1409,10 @@
       <c r="AF8" s="7"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="34"/>
+      <c r="B9" s="54"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -1533,10 +1524,10 @@
       <c r="AF11" s="7"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="34"/>
+      <c r="B12" s="54"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1648,10 +1639,10 @@
       <c r="AF14" s="7"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="34"/>
+      <c r="B15" s="54"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -1763,10 +1754,10 @@
       <c r="AF17" s="7"/>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="54"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -1878,10 +1869,10 @@
       <c r="AF20" s="7"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="34"/>
+      <c r="B21" s="54"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -1993,10 +1984,10 @@
       <c r="AF23" s="7"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="54"/>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
@@ -2027,10 +2018,10 @@
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="34"/>
+      <c r="B27" s="54"/>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
@@ -2130,7 +2121,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" ht="264.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2147,7 +2138,8 @@
   <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <pane ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2162,13 +2154,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="A1" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
@@ -2178,59 +2170,59 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="23"/>
       <c r="C3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="25"/>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="50"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="48"/>
+    </row>
+    <row r="7" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="56"/>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="52.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="51"/>
+      <c r="B8" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="52" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="52"/>
-    </row>
-    <row r="7" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="51" t="s">
+      <c r="E8" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="51"/>
-    </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="52.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
-      <c r="B8" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="56" t="s">
+      <c r="F8" s="52" t="s">
         <v>105</v>
-      </c>
-      <c r="F8" s="56" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
-      <c r="D9" s="36"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2240,7 +2232,7 @@
       <c r="C10" s="15">
         <v>508</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="34">
         <v>0.94074074074074077</v>
       </c>
       <c r="E10" s="16">
@@ -2254,7 +2246,7 @@
       <c r="C11" s="16">
         <v>502</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="35">
         <v>0.92962962962962958</v>
       </c>
     </row>
@@ -2265,7 +2257,7 @@
       <c r="C12" s="16">
         <v>204</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="35">
         <v>0.37777777777777777</v>
       </c>
     </row>
@@ -2276,7 +2268,7 @@
       <c r="C13" s="16">
         <v>180</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="35">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -2287,7 +2279,7 @@
       <c r="C14" s="16">
         <v>177</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="35">
         <v>0.32777777777777778</v>
       </c>
     </row>
@@ -2298,7 +2290,7 @@
       <c r="C15" s="16">
         <v>156</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="35">
         <v>0.28888888888888886</v>
       </c>
     </row>
@@ -2309,7 +2301,7 @@
       <c r="C16" s="16">
         <v>108</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="35">
         <v>0.2</v>
       </c>
     </row>
@@ -2320,7 +2312,7 @@
       <c r="C17" s="16">
         <v>107</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="35">
         <v>0.19814814814814816</v>
       </c>
     </row>
@@ -2331,7 +2323,7 @@
       <c r="C18" s="16">
         <v>105</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="35">
         <v>0.19444444444444445</v>
       </c>
     </row>
@@ -2342,7 +2334,7 @@
       <c r="C19" s="16">
         <v>57</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="35">
         <v>0.10555555555555556</v>
       </c>
     </row>
@@ -2353,7 +2345,7 @@
       <c r="C20" s="16">
         <v>53</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="35">
         <v>9.8148148148148151E-2</v>
       </c>
     </row>
@@ -2364,7 +2356,7 @@
       <c r="C21" s="24">
         <v>52</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="36">
         <v>9.6296296296296297E-2</v>
       </c>
       <c r="F21" s="16">
@@ -2378,7 +2370,7 @@
       <c r="C22" s="24">
         <v>51</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="36">
         <v>9.4444444444444442E-2</v>
       </c>
       <c r="F22" s="16">
@@ -2392,7 +2384,7 @@
       <c r="C23" s="16">
         <v>47</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="35">
         <v>8.7037037037037038E-2</v>
       </c>
     </row>
@@ -2403,7 +2395,7 @@
       <c r="C24" s="15">
         <v>36</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D24" s="34">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="E24" s="16">
@@ -2417,7 +2409,7 @@
       <c r="C25" s="15">
         <v>23</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D25" s="34">
         <v>4.2592592592592592E-2</v>
       </c>
       <c r="E25" s="16">
@@ -2431,7 +2423,7 @@
       <c r="C26" s="15">
         <v>17</v>
       </c>
-      <c r="D26" s="37">
+      <c r="D26" s="34">
         <v>3.1481481481481478E-2</v>
       </c>
       <c r="E26" s="16">
@@ -2445,7 +2437,7 @@
       <c r="C27" s="15">
         <v>13</v>
       </c>
-      <c r="D27" s="37">
+      <c r="D27" s="34">
         <v>2.4074074074074074E-2</v>
       </c>
       <c r="E27" s="16">
@@ -2459,7 +2451,7 @@
       <c r="C28" s="16">
         <v>11</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D28" s="35">
         <v>2.0370370370370372E-2</v>
       </c>
     </row>
@@ -2470,7 +2462,7 @@
       <c r="C29" s="16">
         <v>9</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="35">
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
@@ -2481,7 +2473,7 @@
       <c r="C30" s="15">
         <v>5</v>
       </c>
-      <c r="D30" s="37">
+      <c r="D30" s="34">
         <v>9.2592592592592587E-3</v>
       </c>
       <c r="E30" s="16">
@@ -2495,7 +2487,7 @@
       <c r="C31" s="15">
         <v>3</v>
       </c>
-      <c r="D31" s="37">
+      <c r="D31" s="34">
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="E31" s="16">
@@ -2509,7 +2501,7 @@
       <c r="C32" s="20">
         <v>3</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="37">
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="E32" s="16">
@@ -2521,12 +2513,12 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="46"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="43"/>
     </row>
     <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
@@ -2535,13 +2527,13 @@
       <c r="C34" s="15">
         <v>1049</v>
       </c>
-      <c r="D34" s="37">
+      <c r="D34" s="34">
         <v>0.97129629629629599</v>
       </c>
       <c r="E34" s="16">
         <v>5</v>
       </c>
-      <c r="F34" s="49"/>
+      <c r="F34" s="46"/>
       <c r="H34"/>
     </row>
     <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2551,10 +2543,10 @@
       <c r="C35" s="16">
         <v>1031</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D35" s="35">
         <v>0.95462962962963005</v>
       </c>
-      <c r="F35" s="49"/>
+      <c r="F35" s="46"/>
       <c r="H35"/>
     </row>
     <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2564,13 +2556,13 @@
       <c r="C36" s="15">
         <v>513</v>
       </c>
-      <c r="D36" s="37">
+      <c r="D36" s="34">
         <v>0.47499999999999998</v>
       </c>
       <c r="E36" s="16">
         <v>5</v>
       </c>
-      <c r="F36" s="49"/>
+      <c r="F36" s="46"/>
       <c r="H36"/>
     </row>
     <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2580,10 +2572,10 @@
       <c r="C37" s="16">
         <v>354</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D37" s="35">
         <v>0.327777777777778</v>
       </c>
-      <c r="F37" s="49"/>
+      <c r="F37" s="46"/>
       <c r="H37"/>
     </row>
     <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2593,10 +2585,10 @@
       <c r="C38" s="16">
         <v>329</v>
       </c>
-      <c r="D38" s="38">
+      <c r="D38" s="35">
         <v>0.30462962962963003</v>
       </c>
-      <c r="F38" s="49"/>
+      <c r="F38" s="46"/>
       <c r="H38"/>
     </row>
     <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2606,13 +2598,13 @@
       <c r="C39" s="15">
         <v>233</v>
       </c>
-      <c r="D39" s="37">
+      <c r="D39" s="34">
         <v>0.21574074074074101</v>
       </c>
       <c r="E39" s="16">
         <v>1</v>
       </c>
-      <c r="F39" s="49"/>
+      <c r="F39" s="46"/>
       <c r="H39"/>
     </row>
     <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2622,13 +2614,13 @@
       <c r="C40" s="15">
         <v>179</v>
       </c>
-      <c r="D40" s="37">
+      <c r="D40" s="34">
         <v>0.16574074074074099</v>
       </c>
       <c r="E40" s="16">
         <v>1</v>
       </c>
-      <c r="F40" s="49"/>
+      <c r="F40" s="46"/>
       <c r="H40"/>
     </row>
     <row r="41" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2638,10 +2630,10 @@
       <c r="C41" s="16">
         <v>161</v>
       </c>
-      <c r="D41" s="38">
+      <c r="D41" s="35">
         <v>0.149074074074074</v>
       </c>
-      <c r="F41" s="49"/>
+      <c r="F41" s="46"/>
       <c r="H41"/>
     </row>
     <row r="42" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2651,26 +2643,26 @@
       <c r="C42" s="16">
         <v>142</v>
       </c>
-      <c r="D42" s="38">
+      <c r="D42" s="35">
         <v>0.13148148148148101</v>
       </c>
-      <c r="F42" s="49"/>
+      <c r="F42" s="46"/>
       <c r="H42"/>
     </row>
     <row r="43" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B43" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C43" s="15">
         <v>53</v>
       </c>
-      <c r="D43" s="37">
+      <c r="D43" s="34">
         <v>4.9074074074074103E-2</v>
       </c>
       <c r="E43" s="16">
         <v>4</v>
       </c>
-      <c r="F43" s="49"/>
+      <c r="F43" s="46"/>
       <c r="H43"/>
     </row>
     <row r="44" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2680,13 +2672,13 @@
       <c r="C44" s="20">
         <v>52</v>
       </c>
-      <c r="D44" s="40">
+      <c r="D44" s="37">
         <v>4.81481481481481E-2</v>
       </c>
       <c r="E44" s="16">
         <v>4</v>
       </c>
-      <c r="F44" s="49">
+      <c r="F44" s="46">
         <v>2</v>
       </c>
       <c r="H44"/>
@@ -2698,13 +2690,13 @@
       <c r="C45" s="15">
         <v>51</v>
       </c>
-      <c r="D45" s="37">
+      <c r="D45" s="34">
         <v>4.72222222222222E-2</v>
       </c>
-      <c r="E45" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="49"/>
+      <c r="E45" s="16">
+        <v>4</v>
+      </c>
+      <c r="F45" s="46"/>
       <c r="H45"/>
     </row>
     <row r="46" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2714,13 +2706,12 @@
       <c r="C46" s="24">
         <v>50</v>
       </c>
-      <c r="D46" s="39">
+      <c r="D46" s="36">
         <v>4.6296296296296301E-2</v>
       </c>
-      <c r="E46" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F46" s="49"/>
+      <c r="F46" s="46">
+        <v>5</v>
+      </c>
       <c r="H46"/>
     </row>
     <row r="47" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2730,10 +2721,10 @@
       <c r="C47" s="16">
         <v>49</v>
       </c>
-      <c r="D47" s="38">
+      <c r="D47" s="35">
         <v>4.5370370370370401E-2</v>
       </c>
-      <c r="F47" s="49"/>
+      <c r="F47" s="46"/>
       <c r="H47"/>
     </row>
     <row r="48" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2743,10 +2734,10 @@
       <c r="C48" s="16">
         <v>47</v>
       </c>
-      <c r="D48" s="38">
+      <c r="D48" s="35">
         <v>4.3518518518518498E-2</v>
       </c>
-      <c r="F48" s="49"/>
+      <c r="F48" s="46"/>
       <c r="H48"/>
     </row>
     <row r="49" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2756,29 +2747,29 @@
       <c r="C49" s="15">
         <v>46</v>
       </c>
-      <c r="D49" s="37">
+      <c r="D49" s="34">
         <v>4.2592592592592599E-2</v>
       </c>
-      <c r="E49" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="49"/>
+      <c r="E49" s="16">
+        <v>2</v>
+      </c>
+      <c r="F49" s="46"/>
       <c r="H49"/>
     </row>
     <row r="50" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B50" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C50" s="15">
         <v>31</v>
       </c>
-      <c r="D50" s="37">
+      <c r="D50" s="34">
         <v>2.87037037037037E-2</v>
       </c>
-      <c r="E50" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F50" s="49"/>
+      <c r="E50" s="16">
+        <v>4</v>
+      </c>
+      <c r="F50" s="46"/>
       <c r="H50"/>
     </row>
     <row r="51" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2788,13 +2779,15 @@
       <c r="C51" s="20">
         <v>26</v>
       </c>
-      <c r="D51" s="40">
+      <c r="D51" s="37">
         <v>2.4074074074074098E-2</v>
       </c>
-      <c r="E51" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="F51" s="49"/>
+      <c r="E51" s="16">
+        <v>5</v>
+      </c>
+      <c r="F51" s="46">
+        <v>2</v>
+      </c>
       <c r="H51"/>
     </row>
     <row r="52" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2804,13 +2797,13 @@
       <c r="C52" s="15">
         <v>22</v>
       </c>
-      <c r="D52" s="37">
+      <c r="D52" s="34">
         <v>2.03703703703704E-2</v>
       </c>
-      <c r="E52" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52" s="49"/>
+      <c r="E52" s="16">
+        <v>5</v>
+      </c>
+      <c r="F52" s="46"/>
       <c r="H52"/>
     </row>
     <row r="53" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2820,74 +2813,76 @@
       <c r="C53" s="16">
         <v>21</v>
       </c>
-      <c r="D53" s="38">
+      <c r="D53" s="35">
         <v>1.94444444444444E-2</v>
       </c>
-      <c r="F53" s="49"/>
+      <c r="F53" s="46"/>
       <c r="H53"/>
     </row>
     <row r="54" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B54" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C54" s="20">
         <v>20</v>
       </c>
-      <c r="D54" s="40">
+      <c r="D54" s="37">
         <v>1.85185185185185E-2</v>
       </c>
-      <c r="E54" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F54" s="49"/>
+      <c r="E54" s="16">
+        <v>5</v>
+      </c>
+      <c r="F54" s="46">
+        <v>5</v>
+      </c>
       <c r="H54"/>
     </row>
     <row r="55" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B55" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" s="15">
         <v>15</v>
       </c>
-      <c r="D55" s="37">
+      <c r="D55" s="34">
         <v>1.38888888888889E-2</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F55" s="49"/>
+      <c r="F55" s="46"/>
       <c r="H55"/>
     </row>
     <row r="56" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B56" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" s="15">
         <v>13</v>
       </c>
-      <c r="D56" s="37">
+      <c r="D56" s="34">
         <v>1.2037037037037001E-2</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F56" s="49"/>
+      <c r="F56" s="46"/>
       <c r="H56"/>
     </row>
     <row r="57" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B57" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" s="20">
         <v>12</v>
       </c>
-      <c r="D57" s="40">
+      <c r="D57" s="37">
         <v>1.1111111111111099E-2</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F57" s="49"/>
+      <c r="F57" s="46"/>
       <c r="H57"/>
     </row>
     <row r="58" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2897,45 +2892,45 @@
       <c r="C58" s="32">
         <v>12</v>
       </c>
-      <c r="D58" s="42">
+      <c r="D58" s="39">
         <v>1.1111111111111099E-2</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F58" s="49"/>
+      <c r="F58" s="46"/>
       <c r="H58"/>
     </row>
     <row r="59" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B59" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C59" s="32">
         <v>10</v>
       </c>
-      <c r="D59" s="42">
+      <c r="D59" s="39">
         <v>9.2592592592592605E-3</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="49"/>
+      <c r="F59" s="46"/>
       <c r="H59"/>
     </row>
     <row r="60" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B60" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C60" s="20">
         <v>10</v>
       </c>
-      <c r="D60" s="40">
+      <c r="D60" s="37">
         <v>9.2592592592592605E-3</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F60" s="49"/>
+      <c r="F60" s="46"/>
       <c r="H60"/>
     </row>
     <row r="61" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2945,29 +2940,29 @@
       <c r="C61" s="32">
         <v>8</v>
       </c>
-      <c r="D61" s="42">
+      <c r="D61" s="39">
         <v>7.4074074074074103E-3</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F61" s="49"/>
+      <c r="F61" s="46"/>
       <c r="H61"/>
     </row>
     <row r="62" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B62" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C62" s="20">
         <v>7</v>
       </c>
-      <c r="D62" s="40">
+      <c r="D62" s="37">
         <v>6.4814814814814804E-3</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="F62" s="49"/>
+        <v>100</v>
+      </c>
+      <c r="F62" s="46"/>
       <c r="H62"/>
     </row>
     <row r="63" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2977,13 +2972,13 @@
       <c r="C63" s="20">
         <v>6</v>
       </c>
-      <c r="D63" s="40">
+      <c r="D63" s="37">
         <v>5.5555555555555601E-3</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F63" s="49"/>
+        <v>101</v>
+      </c>
+      <c r="F63" s="46"/>
       <c r="H63"/>
     </row>
     <row r="64" spans="2:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -2993,13 +2988,13 @@
       <c r="C64" s="15">
         <v>3</v>
       </c>
-      <c r="D64" s="37">
+      <c r="D64" s="34">
         <v>2.7777777777777801E-3</v>
       </c>
       <c r="E64" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F64" s="49"/>
+      <c r="F64" s="46"/>
       <c r="H64"/>
     </row>
     <row r="65" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -3009,23 +3004,23 @@
       <c r="C65" s="20">
         <v>2</v>
       </c>
-      <c r="D65" s="40">
+      <c r="D65" s="37">
         <v>1.85185185185185E-3</v>
       </c>
       <c r="E65" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="F65" s="49"/>
+      <c r="F65" s="46"/>
       <c r="H65"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B66" s="18"/>
       <c r="C66" s="17"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="46"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="43"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="27"/>
@@ -3035,7 +3030,7 @@
       <c r="C67" s="16">
         <v>1000</v>
       </c>
-      <c r="D67" s="38">
+      <c r="D67" s="35">
         <v>0.89365504915102767</v>
       </c>
     </row>
@@ -3047,7 +3042,7 @@
       <c r="C68" s="16">
         <v>840</v>
       </c>
-      <c r="D68" s="38">
+      <c r="D68" s="35">
         <v>0.75067024128686322</v>
       </c>
     </row>
@@ -3059,7 +3054,7 @@
       <c r="C69" s="15">
         <v>719</v>
       </c>
-      <c r="D69" s="37">
+      <c r="D69" s="34">
         <v>0.64253798033958887</v>
       </c>
       <c r="E69" s="16" t="s">
@@ -3074,7 +3069,7 @@
       <c r="C70" s="16">
         <v>639</v>
       </c>
-      <c r="D70" s="38">
+      <c r="D70" s="35">
         <v>0.57104557640750675</v>
       </c>
     </row>
@@ -3086,7 +3081,7 @@
       <c r="C71" s="16">
         <v>405</v>
       </c>
-      <c r="D71" s="38">
+      <c r="D71" s="35">
         <v>0.36193029490616624</v>
       </c>
     </row>
@@ -3098,7 +3093,7 @@
       <c r="C72" s="16">
         <v>380</v>
       </c>
-      <c r="D72" s="38">
+      <c r="D72" s="35">
         <v>0.33958891867739055</v>
       </c>
     </row>
@@ -3110,7 +3105,7 @@
       <c r="C73" s="16">
         <v>230</v>
       </c>
-      <c r="D73" s="38">
+      <c r="D73" s="35">
         <v>0.20554066130473636</v>
       </c>
     </row>
@@ -3122,7 +3117,7 @@
       <c r="C74" s="15">
         <v>121</v>
       </c>
-      <c r="D74" s="37">
+      <c r="D74" s="34">
         <v>0.10813226094727435</v>
       </c>
       <c r="E74" s="16" t="s">
@@ -3137,7 +3132,7 @@
       <c r="C75" s="16">
         <v>92</v>
       </c>
-      <c r="D75" s="38">
+      <c r="D75" s="35">
         <v>8.2216264521894553E-2</v>
       </c>
     </row>
@@ -3149,7 +3144,7 @@
       <c r="C76" s="15">
         <v>76</v>
       </c>
-      <c r="D76" s="37">
+      <c r="D76" s="34">
         <v>6.7917783735478104E-2</v>
       </c>
       <c r="E76" s="16" t="s">
@@ -3164,18 +3159,18 @@
       <c r="C77" s="29">
         <v>49</v>
       </c>
-      <c r="D77" s="43">
+      <c r="D77" s="40">
         <v>4.3789097408400354E-2</v>
       </c>
       <c r="E77" s="29"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C78" s="26"/>
-      <c r="D78" s="44"/>
-      <c r="E78" s="47"/>
+      <c r="D78" s="41"/>
+      <c r="E78" s="44"/>
     </row>
     <row r="79" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A79"/>
@@ -3185,10 +3180,10 @@
       <c r="C79" s="16">
         <v>1926</v>
       </c>
-      <c r="D79" s="38">
+      <c r="D79" s="35">
         <v>0.95393759286775603</v>
       </c>
-      <c r="F79" s="49"/>
+      <c r="F79" s="46"/>
       <c r="G79"/>
     </row>
     <row r="80" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -3199,10 +3194,10 @@
       <c r="C80" s="16">
         <v>1419</v>
       </c>
-      <c r="D80" s="38">
+      <c r="D80" s="35">
         <v>0.70282317979197595</v>
       </c>
-      <c r="F80" s="49"/>
+      <c r="F80" s="46"/>
       <c r="G80"/>
     </row>
     <row r="81" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3213,10 +3208,10 @@
       <c r="C81" s="16">
         <v>1233</v>
       </c>
-      <c r="D81" s="38">
+      <c r="D81" s="35">
         <v>0.61069836552748902</v>
       </c>
-      <c r="F81" s="49"/>
+      <c r="F81" s="46"/>
       <c r="G81"/>
     </row>
     <row r="82" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3227,13 +3222,13 @@
       <c r="C82" s="15">
         <v>1128</v>
       </c>
-      <c r="D82" s="37">
+      <c r="D82" s="34">
         <v>0.55869242199108504</v>
       </c>
       <c r="E82" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F82" s="49"/>
+      <c r="F82" s="46"/>
       <c r="G82"/>
     </row>
     <row r="83" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3244,10 +3239,10 @@
       <c r="C83" s="16">
         <v>646</v>
       </c>
-      <c r="D83" s="38">
+      <c r="D83" s="35">
         <v>0.31996037642397201</v>
       </c>
-      <c r="F83" s="49"/>
+      <c r="F83" s="46"/>
       <c r="G83"/>
     </row>
     <row r="84" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3258,10 +3253,10 @@
       <c r="C84" s="16">
         <v>541</v>
       </c>
-      <c r="D84" s="38">
+      <c r="D84" s="35">
         <v>0.26795443288756798</v>
       </c>
-      <c r="F84" s="49"/>
+      <c r="F84" s="46"/>
       <c r="G84"/>
     </row>
     <row r="85" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3272,10 +3267,10 @@
       <c r="C85" s="16">
         <v>313</v>
       </c>
-      <c r="D85" s="38">
+      <c r="D85" s="35">
         <v>0.15502724120851899</v>
       </c>
-      <c r="F85" s="49"/>
+      <c r="F85" s="46"/>
       <c r="G85"/>
     </row>
     <row r="86" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3286,10 +3281,10 @@
       <c r="C86" s="16">
         <v>193</v>
       </c>
-      <c r="D86" s="38">
+      <c r="D86" s="35">
         <v>9.5591877166914294E-2</v>
       </c>
-      <c r="F86" s="49"/>
+      <c r="F86" s="46"/>
       <c r="G86"/>
     </row>
     <row r="87" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3300,10 +3295,10 @@
       <c r="C87" s="16">
         <v>145</v>
       </c>
-      <c r="D87" s="38">
+      <c r="D87" s="35">
         <v>7.1817731550272407E-2</v>
       </c>
-      <c r="F87" s="49"/>
+      <c r="F87" s="46"/>
       <c r="G87"/>
     </row>
     <row r="88" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3314,10 +3309,10 @@
       <c r="C88" s="16">
         <v>73</v>
       </c>
-      <c r="D88" s="38">
+      <c r="D88" s="35">
         <v>3.6156513125309597E-2</v>
       </c>
-      <c r="F88" s="49"/>
+      <c r="F88" s="46"/>
       <c r="G88"/>
     </row>
     <row r="89" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -3328,44 +3323,44 @@
       <c r="C89" s="16">
         <v>56</v>
       </c>
-      <c r="D89" s="38">
+      <c r="D89" s="35">
         <v>2.7736503219415599E-2</v>
       </c>
-      <c r="F89" s="49"/>
+      <c r="F89" s="46"/>
       <c r="G89"/>
     </row>
     <row r="90" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C90" s="15">
         <v>51</v>
       </c>
-      <c r="D90" s="37">
+      <c r="D90" s="34">
         <v>2.5260029717682E-2</v>
       </c>
       <c r="E90" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F90" s="49"/>
+      <c r="F90" s="46"/>
       <c r="G90"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="30"/>
       <c r="B91" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C91" s="31">
         <v>24</v>
       </c>
-      <c r="D91" s="45">
+      <c r="D91" s="42">
         <v>1.1887072808321001E-2</v>
       </c>
-      <c r="E91" s="48" t="s">
+      <c r="E91" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="F91" s="49"/>
+      <c r="F91" s="46"/>
       <c r="G91"/>
     </row>
   </sheetData>

</xml_diff>